<commit_message>
Add data and fixes for 2021 scenario
Signed-off-by: FredericSabot <frederic.sabot@ulb.be>
</commit_message>
<xml_diff>
--- a/FES data/aggregated/SummerPM_30_leading_analysis.xlsx
+++ b/FES data/aggregated/SummerPM_30_leading_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Dropbox\PC\Downloads\CIGRE2024\scripts\FES data\aggregated\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F064A1B6-B8D0-4797-BD36-0A0B287D3549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF6DD2F3-0286-4AA3-B7CD-F1BDFE4C6369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2431,7 +2431,7 @@
   <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>